<commit_message>
first version of first level complete, some minor ui changes
</commit_message>
<xml_diff>
--- a/cards/card_spreadsheet.xlsx
+++ b/cards/card_spreadsheet.xlsx
@@ -271,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -280,7 +280,6 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -684,10 +683,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E409D199-6017-4BC2-A752-B58E23564277}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +698,7 @@
     <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -716,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>29</v>
       </c>
@@ -733,7 +732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>51</v>
       </c>
@@ -750,7 +749,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -767,7 +766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>45</v>
       </c>
@@ -784,7 +783,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -801,7 +800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
@@ -818,7 +817,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -835,7 +834,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -852,7 +851,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
@@ -869,7 +868,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -886,7 +885,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>53</v>
       </c>
@@ -903,7 +902,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>32</v>
       </c>
@@ -920,7 +919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>49</v>
       </c>
@@ -936,9 +935,8 @@
       <c r="E14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>46</v>
       </c>
@@ -955,7 +953,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -972,7 +970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -989,7 +987,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>43</v>
       </c>
@@ -1006,7 +1004,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>27</v>
       </c>
@@ -1023,7 +1021,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -1040,7 +1038,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>56</v>
       </c>
@@ -1056,7 +1054,6 @@
       <c r="E21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E21" xr:uid="{E409D199-6017-4BC2-A752-B58E23564277}">

</xml_diff>